<commit_message>
Done update user profile
</commit_message>
<xml_diff>
--- a/src/data/Project-Controller.xlsx
+++ b/src/data/Project-Controller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bes/cc18/Project/Swapy02/web/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E88D6BA-B843-4045-96F1-F1280ECAE3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C4C490-13C4-994C-8932-46A8141B516D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4940" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="8" xr2:uid="{EBC99A39-14E9-FD43-AB84-C80166CFC4A2}"/>
+    <workbookView xWindow="28800" yWindow="2100" windowWidth="23600" windowHeight="15900" activeTab="8" xr2:uid="{EBC99A39-14E9-FD43-AB84-C80166CFC4A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="22" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Assets!$A$1:$N$195</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">WBS!$A$2:$AG$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">WBS!$A$2:$AG$103</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24843,16 +24843,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F0E61F-A3F6-9740-95CC-82129F9B310C}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:AG103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="H45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="L49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG52" sqref="AG52"/>
+      <selection pane="bottomRight" activeCell="AG54" sqref="AG54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24881,7 +24881,7 @@
       </c>
       <c r="AG1" s="20" cm="1">
         <f t="array" ref="AG1">SUM($G$3:$G$1024*$AG$3:$AG$1024)/G1</f>
-        <v>0.62240000000000018</v>
+        <v>0.63040000000000018</v>
       </c>
     </row>
     <row r="2" spans="1:33" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -24985,7 +24985,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -25011,7 +25011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <f t="shared" ref="A4:A68" si="0">IF(B4=1,A3+1,A3)</f>
         <v>1</v>
@@ -25038,7 +25038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -25065,7 +25065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -25092,7 +25092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25122,7 +25122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25152,7 +25152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25182,7 +25182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25212,7 +25212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25242,7 +25242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25272,7 +25272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25302,7 +25302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25332,7 +25332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25362,7 +25362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25392,7 +25392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25422,7 +25422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25452,7 +25452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -25482,7 +25482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -25512,7 +25512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -25542,7 +25542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -25572,7 +25572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -25602,7 +25602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -25632,7 +25632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -25662,7 +25662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -25689,7 +25689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -25716,7 +25716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -25743,7 +25743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -25773,7 +25773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -25803,7 +25803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -25833,7 +25833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -25863,7 +25863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -25893,7 +25893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:33" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -25923,7 +25923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -25953,7 +25953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -25983,7 +25983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -26013,7 +26013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -26040,7 +26040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -26067,7 +26067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -26094,7 +26094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -26121,7 +26121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -26148,7 +26148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -26178,7 +26178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -26208,7 +26208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -26238,7 +26238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -26268,7 +26268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -26298,7 +26298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -26349,13 +26349,13 @@
         <v>1225</v>
       </c>
       <c r="S49" s="15" t="s">
-        <v>1346</v>
+        <v>1227</v>
       </c>
       <c r="AG49" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -26388,7 +26388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -26418,7 +26418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -26448,7 +26448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -26544,7 +26544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -26697,7 +26697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -26727,7 +26727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -26757,7 +26757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -26787,7 +26787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -26817,7 +26817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -26847,7 +26847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -26877,7 +26877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -26907,7 +26907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -26937,7 +26937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="15">
         <f t="shared" ref="A69:A103" si="1">IF(B69=1,A68+1,A68)</f>
         <v>7</v>
@@ -26967,7 +26967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -26997,7 +26997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27027,7 +27027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27057,7 +27057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27087,7 +27087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27114,7 +27114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27141,7 +27141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27168,7 +27168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27195,7 +27195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27222,7 +27222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27249,7 +27249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27276,7 +27276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27303,7 +27303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27330,7 +27330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27357,7 +27357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -27384,7 +27384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -27417,7 +27417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -27450,7 +27450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -27483,7 +27483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -27516,7 +27516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -27549,7 +27549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -27579,7 +27579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -27609,7 +27609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -27639,7 +27639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -27672,7 +27672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -27834,7 +27834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="15">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -27864,7 +27864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="15">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -27894,7 +27894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:33" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:33" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="15">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -27985,7 +27985,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AG101" xr:uid="{63F0E61F-A3F6-9740-95CC-82129F9B310C}"/>
+  <autoFilter ref="A2:AG103" xr:uid="{63F0E61F-A3F6-9740-95CC-82129F9B310C}">
+    <filterColumn colId="32">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="H1:AF1048576">
     <cfRule type="expression" dxfId="5" priority="1">
       <formula>H1="O"</formula>

</xml_diff>